<commit_message>
Added some Android-Build-Files | Added Things for Presentation
</commit_message>
<xml_diff>
--- a/Präsentation/Planung.xlsx
+++ b/Präsentation/Planung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgaben" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Aufgabenliste "Gruppenprojekt"</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>nicht begonnen</t>
-  </si>
-  <si>
     <t>Notizen</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>hoch</t>
   </si>
   <si>
-    <t>mittel</t>
-  </si>
-  <si>
     <t>niedrig</t>
   </si>
   <si>
@@ -101,12 +95,6 @@
     <t>Plakate erstellen</t>
   </si>
   <si>
-    <t>Standdesign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kommentare &amp; IF-Abfragen hinzufügen </t>
-  </si>
-  <si>
     <t>Projektleitung</t>
   </si>
   <si>
@@ -114,6 +102,27 @@
   </si>
   <si>
     <t>zusammen</t>
+  </si>
+  <si>
+    <t>in Bearbeitung</t>
+  </si>
+  <si>
+    <t>-&gt; Überlegen, welche Fragen gestellt werden könnten</t>
+  </si>
+  <si>
+    <t>-&gt; Grundlegendes Design für Plakate usw.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; Kommentare &amp; IF-Abfragen hinzufügen </t>
+  </si>
+  <si>
+    <t>-&gt; Java-Video fehlt</t>
+  </si>
+  <si>
+    <t>Standdesign und Ablaufplanung</t>
+  </si>
+  <si>
+    <t>-&gt; Fertig geplant: drucken</t>
   </si>
 </sst>
 </file>
@@ -123,10 +132,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-407]d/\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.14993743705557422"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,13 +184,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.249977111117893"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Tahoma"/>
@@ -196,41 +205,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.14993743705557422"/>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.249977111117893"/>
-      <name val="Tahoma"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +246,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -292,24 +280,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -318,55 +307,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
+    <cellStyle name="60 % - Akzent2" xfId="9" builtinId="36"/>
     <cellStyle name="Gut" xfId="6" builtinId="26"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27"/>
@@ -377,119 +361,7 @@
     <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -521,9 +393,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1" tint="0.249977111117893"/>
         <name val="Tahoma"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -532,6 +405,17 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -554,6 +438,203 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -602,12 +683,17 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Liste &quot;Gruppenprojekt&quot;" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Liste &quot;Gruppenprojekt&quot;" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstColumn" dxfId="23"/>
+      <tableStyleElement type="wholeTable" dxfId="39"/>
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="totalRow" dxfId="37"/>
+      <tableStyleElement type="firstColumn" dxfId="36"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF9F3160"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -620,18 +706,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="B6:G13" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="B6:G13" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="B6:G13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="B7:G15">
-    <sortCondition ref="E6:E15"/>
+  <sortState ref="B7:G13">
+    <sortCondition descending="1" ref="F6:F13"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Zuständiger" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priorität" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Zieldatum" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Notizen" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aufgaben" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Zuständiger" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priorität" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Zieldatum" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Notizen" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Liste &quot;Gruppenprojekt&quot;" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -909,10 +995,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -940,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4" t="s">
@@ -949,14 +1035,14 @@
       <c r="G3"/>
     </row>
     <row r="4" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12">
+      <c r="D4" s="10"/>
+      <c r="E4" s="11">
         <v>43151</v>
       </c>
       <c r="G4"/>
@@ -970,9 +1056,9 @@
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -982,200 +1068,186 @@
         <v>6</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="2">
-        <v>43114</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="3" t="s">
+        <v>43131</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>25</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2">
-        <v>43116</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>22</v>
+        <v>43145</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="2">
-        <v>43115</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>22</v>
+        <v>43125</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="12">
+        <v>43129</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2">
-        <v>43125</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="2">
-        <v>43129</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>7</v>
+        <v>43114</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2">
+        <v>43116</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2">
-        <v>43145</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E13" s="2">
         <v>43138</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="13"/>
-      <c r="F15" s="7"/>
+      <c r="F13" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F15 F7:F9 F11:F13">
-    <cfRule type="expression" dxfId="15" priority="15">
-      <formula>UPPER(F7)="nicht begonnen"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
-      <formula>UPPER(F7)="in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>UPPER(F7)="erledigt"</formula>
+  <conditionalFormatting sqref="F13 F11">
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>UPPER(F11)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>UPPER(F11)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>UPPER(F11)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="mittel">
-      <formula>NOT(ISERROR(SEARCH("mittel",D12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="sehr hoch">
-      <formula>NOT(ISERROR(SEARCH("sehr hoch",D12)))</formula>
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="niedrig">
+      <formula>NOT(ISERROR(SEARCH("niedrig",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="niedrig">
-      <formula>NOT(ISERROR(SEARCH("niedrig",D14)))</formula>
+  <conditionalFormatting sqref="C10:C11 C7:C8">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Vincent">
+      <formula>NOT(ISERROR(SEARCH("Vincent",C7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Fabian">
+      <formula>NOT(ISERROR(SEARCH("Fabian",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C9 C11:C13">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Vincent">
-      <formula>NOT(ISERROR(SEARCH("Vincent",C7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Fabian">
-      <formula>NOT(ISERROR(SEARCH("Fabian",C7)))</formula>
+  <conditionalFormatting sqref="D10:D12 D7:D8">
+    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="mittel">
+      <formula>NOT(ISERROR(SEARCH("mittel",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="dauerhafte Aufgabe">
-      <formula>NOT(ISERROR(SEARCH("dauerhafte Aufgabe",F14)))</formula>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="hoch">
+      <formula>NOT(ISERROR(SEARCH("hoch",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D9 D11:D14">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="mittel">
-      <formula>NOT(ISERROR(SEARCH("mittel",D7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="hoch">
-      <formula>NOT(ISERROR(SEARCH("hoch",D9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="4" priority="27" operator="containsText" text="mittel">
-      <formula>NOT(ISERROR(SEARCH("mittel",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="28" operator="containsText" text="hoch">
-      <formula>NOT(ISERROR(SEARCH("hoch",D13)))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="29">
+  <conditionalFormatting sqref="D11">
+    <cfRule type="containsText" dxfId="27" priority="49" operator="containsText" text="mittel">
+      <formula>NOT(ISERROR(SEARCH("mittel",D11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="50" operator="containsText" text="hoch">
+      <formula>NOT(ISERROR(SEARCH("hoch",D11)))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1186,15 +1258,77 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="expression" dxfId="25" priority="23">
+      <formula>UPPER(F9)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="24">
+      <formula>UPPER(F9)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="25">
+      <formula>UPPER(F9)="erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="Vincent">
+      <formula>NOT(ISERROR(SEARCH("Vincent",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="Fabian">
+      <formula>NOT(ISERROR(SEARCH("Fabian",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="expression" dxfId="20" priority="15">
+      <formula>UPPER(F12)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="16">
+      <formula>UPPER(F12)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="17">
+      <formula>UPPER(F12)="erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="17" priority="12">
+      <formula>UPPER(F10)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="13">
+      <formula>UPPER(F10)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="14">
+      <formula>UPPER(F10)="erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="niedrig">
+      <formula>NOT(ISERROR(SEARCH("niedrig",D13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="mittel">
+      <formula>NOT(ISERROR(SEARCH("mittel",D13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" dxfId="12" priority="7">
+      <formula>UPPER(F8)="nicht begonnen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="8">
+      <formula>UPPER(F8)="in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="9">
+      <formula>UPPER(F8)="erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>UPPER(F10)="nicht begonnen"</formula>
+      <formula>UPPER(F7)="nicht begonnen"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>UPPER(F10)="in Bearbeitung"</formula>
+      <formula>UPPER(F7)="in Bearbeitung"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>UPPER(F10)="erledigt"</formula>
+      <formula>UPPER(F7)="erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>